<commit_message>
Finish interface planilla haberes create
</commit_message>
<xml_diff>
--- a/Arch_help/campos_planillas_haberes.xlsx
+++ b/Arch_help/campos_planillas_haberes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProyectosLaravel\LaravelTest\Arch_help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD4AF36-23FB-4F9B-BA0B-6A27C9240A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21BA7FE-9BC7-447B-A477-4CD30F9C8F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="2625" windowWidth="23895" windowHeight="6360" activeTab="2" xr2:uid="{4933B99E-22D6-45F2-87A4-D6553ED4FDCB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4933B99E-22D6-45F2-87A4-D6553ED4FDCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Campos por años" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">limpieza_tabla_rem!$A$1:$A$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="585">
   <si>
     <t>REMUNERACIONES</t>
   </si>
@@ -1009,9 +1008,6 @@
     <t>bon_frontera</t>
   </si>
   <si>
-    <t>bon_comp_serv</t>
-  </si>
-  <si>
     <t>costo_vida</t>
   </si>
   <si>
@@ -1163,6 +1159,645 @@
   </si>
   <si>
     <t>rem_basico</t>
+  </si>
+  <si>
+    <t>rh_aguinaldo</t>
+  </si>
+  <si>
+    <t>rh_al_cargo</t>
+  </si>
+  <si>
+    <t>rh_bon_anos_servicio</t>
+  </si>
+  <si>
+    <t>rh_bon_frontera</t>
+  </si>
+  <si>
+    <t>rh_costo_vida</t>
+  </si>
+  <si>
+    <t>rh_dedicac_exclusiva</t>
+  </si>
+  <si>
+    <t>rh_especializacion_especial</t>
+  </si>
+  <si>
+    <t>rh_familia</t>
+  </si>
+  <si>
+    <t>rh_familia_numerosa</t>
+  </si>
+  <si>
+    <t>rh_fonavi</t>
+  </si>
+  <si>
+    <t>rh_fondo_est</t>
+  </si>
+  <si>
+    <t>rh_gastos_representacion</t>
+  </si>
+  <si>
+    <t>rh_gratificacion</t>
+  </si>
+  <si>
+    <t>rh_gratificacion_altura</t>
+  </si>
+  <si>
+    <t>rh_inc_afp</t>
+  </si>
+  <si>
+    <t>rh_micro</t>
+  </si>
+  <si>
+    <t>rh_personal</t>
+  </si>
+  <si>
+    <t>rh_refri y movil</t>
+  </si>
+  <si>
+    <t>rh_reintegro</t>
+  </si>
+  <si>
+    <t>rh_reunific</t>
+  </si>
+  <si>
+    <t>rh_s_eventual</t>
+  </si>
+  <si>
+    <t>rh_t no pensionable</t>
+  </si>
+  <si>
+    <t>rh_t_pensionable</t>
+  </si>
+  <si>
+    <t>rh_t_homol</t>
+  </si>
+  <si>
+    <t>rh_tiempo de servicio</t>
+  </si>
+  <si>
+    <t>rh_viaticos</t>
+  </si>
+  <si>
+    <t>rh_ley_13455</t>
+  </si>
+  <si>
+    <t>rh_ley_13455_16710</t>
+  </si>
+  <si>
+    <t>rh_ley_26504</t>
+  </si>
+  <si>
+    <t>rh_dl_21394</t>
+  </si>
+  <si>
+    <t>rh_dl_25697</t>
+  </si>
+  <si>
+    <t>rh_dl_25897</t>
+  </si>
+  <si>
+    <t>rh_dl_26504</t>
+  </si>
+  <si>
+    <t>rh_dl_31394</t>
+  </si>
+  <si>
+    <t>rh_dl_21899_21394</t>
+  </si>
+  <si>
+    <t>rh_ds_25759</t>
+  </si>
+  <si>
+    <t>rh_ds_3887</t>
+  </si>
+  <si>
+    <t>rh_ds_03188</t>
+  </si>
+  <si>
+    <t>rh_ds_15588</t>
+  </si>
+  <si>
+    <t>rh_ds_13289</t>
+  </si>
+  <si>
+    <t>rh_ds_28589</t>
+  </si>
+  <si>
+    <t>rh_ds_05191</t>
+  </si>
+  <si>
+    <t>rh_ds_27691</t>
+  </si>
+  <si>
+    <t>rh_du_3794</t>
+  </si>
+  <si>
+    <t>rh_du_9096</t>
+  </si>
+  <si>
+    <t>rh_ds_25697</t>
+  </si>
+  <si>
+    <t>rh_du_7397</t>
+  </si>
+  <si>
+    <t>rh_du_01199</t>
+  </si>
+  <si>
+    <t>rh_ds_1605</t>
+  </si>
+  <si>
+    <t>rh_ds_1705</t>
+  </si>
+  <si>
+    <t>rh_ds_11006</t>
+  </si>
+  <si>
+    <t>rh_ds_3907</t>
+  </si>
+  <si>
+    <t>rh_ds_12008</t>
+  </si>
+  <si>
+    <t>rh_ds_1409</t>
+  </si>
+  <si>
+    <t>adelanto_sueldo</t>
+  </si>
+  <si>
+    <t>aporte_afp</t>
+  </si>
+  <si>
+    <t>buena_cuenta</t>
+  </si>
+  <si>
+    <t>cuarta_cat</t>
+  </si>
+  <si>
+    <t>derrama_adm</t>
+  </si>
+  <si>
+    <t>dev_afp</t>
+  </si>
+  <si>
+    <t>fondo_spp</t>
+  </si>
+  <si>
+    <t>quinta_cat</t>
+  </si>
+  <si>
+    <t>pll_afp</t>
+  </si>
+  <si>
+    <t>r_afp</t>
+  </si>
+  <si>
+    <t>imp_rent</t>
+  </si>
+  <si>
+    <t>prestamo_adm</t>
+  </si>
+  <si>
+    <t>snp_5</t>
+  </si>
+  <si>
+    <t>judicial</t>
+  </si>
+  <si>
+    <t>voluntario</t>
+  </si>
+  <si>
+    <t>fonavi_1</t>
+  </si>
+  <si>
+    <t>fondo</t>
+  </si>
+  <si>
+    <t>fonavi_05</t>
+  </si>
+  <si>
+    <t>fondo_10</t>
+  </si>
+  <si>
+    <t>fondo_spp_8</t>
+  </si>
+  <si>
+    <t>snp</t>
+  </si>
+  <si>
+    <t>snp_25</t>
+  </si>
+  <si>
+    <t>snp_3</t>
+  </si>
+  <si>
+    <t>snp_11</t>
+  </si>
+  <si>
+    <t>snp_13</t>
+  </si>
+  <si>
+    <t>goce_6</t>
+  </si>
+  <si>
+    <t>goce_8</t>
+  </si>
+  <si>
+    <t>ips</t>
+  </si>
+  <si>
+    <t>ips_25</t>
+  </si>
+  <si>
+    <t>ips_3</t>
+  </si>
+  <si>
+    <t>ips_4</t>
+  </si>
+  <si>
+    <t>montepio</t>
+  </si>
+  <si>
+    <t>quincena</t>
+  </si>
+  <si>
+    <t>tesoreria</t>
+  </si>
+  <si>
+    <t>ley_7904</t>
+  </si>
+  <si>
+    <t>dl_20530</t>
+  </si>
+  <si>
+    <t>dl_22161</t>
+  </si>
+  <si>
+    <t>ds_043</t>
+  </si>
+  <si>
+    <t>caja_pen</t>
+  </si>
+  <si>
+    <t>caja_pen_1</t>
+  </si>
+  <si>
+    <t>caja_pen_3</t>
+  </si>
+  <si>
+    <t>falta_tard</t>
+  </si>
+  <si>
+    <t>fondo_pen_6</t>
+  </si>
+  <si>
+    <t>fondo_pen_847</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>ret_afp</t>
+  </si>
+  <si>
+    <t>grati</t>
+  </si>
+  <si>
+    <t>snp_2</t>
+  </si>
+  <si>
+    <t>grav_nomb</t>
+  </si>
+  <si>
+    <t>imp_sueldo</t>
+  </si>
+  <si>
+    <t>seg_soc</t>
+  </si>
+  <si>
+    <t>seg_soc_15</t>
+  </si>
+  <si>
+    <t>seg_soc_21</t>
+  </si>
+  <si>
+    <t>seg_soc_25</t>
+  </si>
+  <si>
+    <t>seg_vida</t>
+  </si>
+  <si>
+    <t>vacac</t>
+  </si>
+  <si>
+    <t>comp_serv</t>
+  </si>
+  <si>
+    <t>rh_comp_serv</t>
+  </si>
+  <si>
+    <t>Adelanto Sueldo</t>
+  </si>
+  <si>
+    <t>Buena Cuenta</t>
+  </si>
+  <si>
+    <t>Cuarta Cat</t>
+  </si>
+  <si>
+    <t>Quinta Cat</t>
+  </si>
+  <si>
+    <t>Derrama Adm</t>
+  </si>
+  <si>
+    <t>Desc Vol</t>
+  </si>
+  <si>
+    <t>Fon 1%</t>
+  </si>
+  <si>
+    <t>Fonavi</t>
+  </si>
+  <si>
+    <t>Fonavi 0.5%</t>
+  </si>
+  <si>
+    <t>Fondo</t>
+  </si>
+  <si>
+    <t>Fondo 10%</t>
+  </si>
+  <si>
+    <t>Fondo Pensiones 6%</t>
+  </si>
+  <si>
+    <t>Fondo Pensiones 8-4-7%</t>
+  </si>
+  <si>
+    <t>Fondo Spp 8%</t>
+  </si>
+  <si>
+    <t>Fondo-Spp</t>
+  </si>
+  <si>
+    <t>Aporte Afp</t>
+  </si>
+  <si>
+    <t>Dev Afp</t>
+  </si>
+  <si>
+    <t>Pll Afp</t>
+  </si>
+  <si>
+    <t>R Afp</t>
+  </si>
+  <si>
+    <t>Retencion</t>
+  </si>
+  <si>
+    <t>Retencion Afp</t>
+  </si>
+  <si>
+    <t>Snp</t>
+  </si>
+  <si>
+    <t>Snp 2%</t>
+  </si>
+  <si>
+    <t>Snp 2.5%</t>
+  </si>
+  <si>
+    <t>Snp 3%</t>
+  </si>
+  <si>
+    <t>Snp 11%</t>
+  </si>
+  <si>
+    <t>Snp 13%</t>
+  </si>
+  <si>
+    <t>Goce 6%</t>
+  </si>
+  <si>
+    <t>Goce 8%</t>
+  </si>
+  <si>
+    <t>Gratificacion</t>
+  </si>
+  <si>
+    <t>Grav Nombram</t>
+  </si>
+  <si>
+    <t>Imp Rent</t>
+  </si>
+  <si>
+    <t>Impuesto Sueldo</t>
+  </si>
+  <si>
+    <t>Ips</t>
+  </si>
+  <si>
+    <t>Ips 2.5%</t>
+  </si>
+  <si>
+    <t>Ips 3%</t>
+  </si>
+  <si>
+    <t>Ips 4%</t>
+  </si>
+  <si>
+    <t>Montepio</t>
+  </si>
+  <si>
+    <t>Prestamo Adm</t>
+  </si>
+  <si>
+    <t>Quincena</t>
+  </si>
+  <si>
+    <t>Seguro Vida</t>
+  </si>
+  <si>
+    <t>Tesoreria</t>
+  </si>
+  <si>
+    <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>Viaticos</t>
+  </si>
+  <si>
+    <t>Ley 7904</t>
+  </si>
+  <si>
+    <t>Dl 20530</t>
+  </si>
+  <si>
+    <t>Dl 22161</t>
+  </si>
+  <si>
+    <t>Ds 043</t>
+  </si>
+  <si>
+    <t>Caja Pension 1%</t>
+  </si>
+  <si>
+    <t>Caja Pension</t>
+  </si>
+  <si>
+    <t>Caja Pension 3%</t>
+  </si>
+  <si>
+    <t>Desc. Judicial</t>
+  </si>
+  <si>
+    <t>Falta Y Tard</t>
+  </si>
+  <si>
+    <t>Seguro Soc</t>
+  </si>
+  <si>
+    <t>Seguro Soc 1.5%</t>
+  </si>
+  <si>
+    <t>Seguro Soc 2.1%</t>
+  </si>
+  <si>
+    <t>Seguro Soc 2.5%</t>
+  </si>
+  <si>
+    <t>Caja Pens</t>
+  </si>
+  <si>
+    <t>Cem 3%</t>
+  </si>
+  <si>
+    <t>Cem 5%</t>
+  </si>
+  <si>
+    <t>Cen</t>
+  </si>
+  <si>
+    <t>Cen 5%</t>
+  </si>
+  <si>
+    <t>Cen 6%</t>
+  </si>
+  <si>
+    <t>Seg Soc</t>
+  </si>
+  <si>
+    <t>Essalud 9%</t>
+  </si>
+  <si>
+    <t>Fon 4%</t>
+  </si>
+  <si>
+    <t>Fon 5%</t>
+  </si>
+  <si>
+    <t>Fon 8%</t>
+  </si>
+  <si>
+    <t>Fon 9%</t>
+  </si>
+  <si>
+    <t>Fon 7%</t>
+  </si>
+  <si>
+    <t>Ipss</t>
+  </si>
+  <si>
+    <t>Ies 1.7%</t>
+  </si>
+  <si>
+    <t>Ies 2%</t>
+  </si>
+  <si>
+    <t>Ipss 6%</t>
+  </si>
+  <si>
+    <t>Ipss 9%</t>
+  </si>
+  <si>
+    <t>Snp 5%</t>
+  </si>
+  <si>
+    <t>Snp 6%</t>
+  </si>
+  <si>
+    <t>Ss Cuota Pat</t>
+  </si>
+  <si>
+    <t>Cp Cuota Pat</t>
+  </si>
+  <si>
+    <t>ss_cuota_pat</t>
+  </si>
+  <si>
+    <t>cp_cuota_pat</t>
+  </si>
+  <si>
+    <t>caja_pens</t>
+  </si>
+  <si>
+    <t>cem_3</t>
+  </si>
+  <si>
+    <t>cem_5</t>
+  </si>
+  <si>
+    <t>cen_5</t>
+  </si>
+  <si>
+    <t>cen_6</t>
+  </si>
+  <si>
+    <t>essalud_9</t>
+  </si>
+  <si>
+    <t>fon_4</t>
+  </si>
+  <si>
+    <t>fon_5</t>
+  </si>
+  <si>
+    <t>fon_8</t>
+  </si>
+  <si>
+    <t>fon_9</t>
+  </si>
+  <si>
+    <t>fon_7</t>
+  </si>
+  <si>
+    <t>ies_7</t>
+  </si>
+  <si>
+    <t>ies_2</t>
+  </si>
+  <si>
+    <t>ipss_6</t>
+  </si>
+  <si>
+    <t>ipss_9</t>
+  </si>
+  <si>
+    <t>snp_6</t>
+  </si>
+  <si>
+    <t>cen</t>
+  </si>
+  <si>
+    <t>ipss</t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -1534,6 +2169,7 @@
       <font>
         <b/>
         <i val="0"/>
+        <strike val="0"/>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
@@ -1541,7 +2177,6 @@
       <font>
         <b/>
         <i val="0"/>
-        <strike val="0"/>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
@@ -1864,11 +2499,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D341C7-600F-4905-B7A0-ABBE51A9946C}">
   <dimension ref="A1:EY68"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="DF24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="DP37" sqref="DP37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -6983,10 +7618,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A3D1FCB-D716-4341-A53F-3D2976AC7945}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6996,9 +7631,10 @@
     <col min="3" max="4" width="27.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>288</v>
       </c>
@@ -7007,7 +7643,7 @@
       </c>
       <c r="D1" s="32"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>112</v>
       </c>
@@ -7022,10 +7658,13 @@
         <v>316</v>
       </c>
       <c r="F2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+      <c r="G2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>85</v>
       </c>
@@ -7043,8 +7682,11 @@
         <f>_xlfn.CONCAT("r_",E3)</f>
         <v>r_aguinaldo</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>6</v>
       </c>
@@ -7062,8 +7704,11 @@
         <f>_xlfn.CONCAT("r_",E4)</f>
         <v>r_al_cargo</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>11</v>
       </c>
@@ -7078,11 +7723,14 @@
         <v>319</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F57" si="1">_xlfn.CONCAT("r_",E5)</f>
+        <f t="shared" ref="F5:G57" si="1">_xlfn.CONCAT("r_",E5)</f>
         <v>r_bon_anos_servicio</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>12</v>
       </c>
@@ -7100,8 +7748,11 @@
         <f t="shared" si="1"/>
         <v>r_bon_frontera</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>71</v>
       </c>
@@ -7113,14 +7764,17 @@
         <v>Compensacion Viv</v>
       </c>
       <c r="E7" t="s">
-        <v>321</v>
+        <v>482</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>r_bon_comp_serv</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>r_comp_serv</v>
+      </c>
+      <c r="G7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>71</v>
       </c>
@@ -7132,14 +7786,17 @@
         <v>Costo Vida</v>
       </c>
       <c r="E8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
         <v>r_costo_vida</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>56</v>
       </c>
@@ -7151,14 +7808,17 @@
         <v>Dedicac Exclusiva</v>
       </c>
       <c r="E9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
         <v>r_dedicac_exclusiva</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>106</v>
       </c>
@@ -7170,14 +7830,17 @@
         <v>Especializacion / Especial</v>
       </c>
       <c r="E10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
         <v>r_especializacion_especial</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>108</v>
       </c>
@@ -7189,14 +7852,17 @@
         <v>Familia</v>
       </c>
       <c r="E11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
         <v>r_familia</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>209</v>
       </c>
@@ -7208,14 +7874,17 @@
         <v>Familia Numerosa</v>
       </c>
       <c r="E12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
         <v>r_familia_numerosa</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>254</v>
       </c>
@@ -7227,14 +7896,17 @@
         <v>Fonavi</v>
       </c>
       <c r="E13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
         <v>r_fonavi</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>256</v>
       </c>
@@ -7246,14 +7918,17 @@
         <v>Fondo Est</v>
       </c>
       <c r="E14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
         <v>r_fondo_est</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>104</v>
       </c>
@@ -7265,14 +7940,17 @@
         <v>Gastos Representacion</v>
       </c>
       <c r="E15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
         <v>r_gastos_representacion</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>176</v>
       </c>
@@ -7284,14 +7962,17 @@
         <v>Gratificacion</v>
       </c>
       <c r="E16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
         <v>r_gratificacion</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>291</v>
       </c>
@@ -7303,14 +7984,17 @@
         <v>Gratificacion Altura</v>
       </c>
       <c r="E17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
         <v>r_gratificacion_altura</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>291</v>
       </c>
@@ -7322,14 +8006,17 @@
         <v>Inc Afp</v>
       </c>
       <c r="E18" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
         <v>r_inc_afp</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>292</v>
       </c>
@@ -7341,14 +8028,17 @@
         <v>Micro</v>
       </c>
       <c r="E19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
         <v>r_micro</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>293</v>
       </c>
@@ -7360,14 +8050,17 @@
         <v>Personal</v>
       </c>
       <c r="E20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
         <v>r_personal</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>181</v>
       </c>
@@ -7379,14 +8072,17 @@
         <v>Refri Y Movil</v>
       </c>
       <c r="E21" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
         <v>r_refri y movil</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>294</v>
       </c>
@@ -7398,14 +8094,17 @@
         <v>Reintegro</v>
       </c>
       <c r="E22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
         <v>r_reintegro</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>174</v>
       </c>
@@ -7417,14 +8116,17 @@
         <v>Reunific</v>
       </c>
       <c r="E23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
         <v>r_reunific</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>295</v>
       </c>
@@ -7436,14 +8138,17 @@
         <v>S Eventual</v>
       </c>
       <c r="E24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
         <v>r_s_eventual</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>296</v>
       </c>
@@ -7455,14 +8160,17 @@
         <v>T No Pensionable</v>
       </c>
       <c r="E25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
         <v>r_t no pensionable</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>297</v>
       </c>
@@ -7474,14 +8182,17 @@
         <v>T Pensionable</v>
       </c>
       <c r="E26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
         <v>r_t_pensionable</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>298</v>
       </c>
@@ -7493,14 +8204,17 @@
         <v>T Homol</v>
       </c>
       <c r="E27" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
         <v>r_t_homol</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>305</v>
       </c>
@@ -7512,14 +8226,17 @@
         <v>Tiempo De Servicio</v>
       </c>
       <c r="E28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
         <v>r_tiempo de servicio</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>172</v>
       </c>
@@ -7531,14 +8248,17 @@
         <v>Viaticos</v>
       </c>
       <c r="E29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
         <v>r_viaticos</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>299</v>
       </c>
@@ -7550,14 +8270,17 @@
         <v>Ley 13455</v>
       </c>
       <c r="E30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
         <v>r_ley_13455</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>300</v>
       </c>
@@ -7569,14 +8292,17 @@
         <v>Ley 13455 Y 16710</v>
       </c>
       <c r="E31" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
         <v>r_ley_13455_16710</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>301</v>
       </c>
@@ -7588,14 +8314,17 @@
         <v>Ley 26504</v>
       </c>
       <c r="E32" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
         <v>r_ley_26504</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>302</v>
       </c>
@@ -7607,14 +8336,17 @@
         <v>Dl 21394</v>
       </c>
       <c r="E33" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
         <v>r_dl_21394</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>303</v>
       </c>
@@ -7626,14 +8358,17 @@
         <v>Dl 25697</v>
       </c>
       <c r="E34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
         <v>r_dl_25697</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>304</v>
       </c>
@@ -7645,14 +8380,17 @@
         <v>Dl 25897</v>
       </c>
       <c r="E35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
         <v>r_dl_25897</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
         <v>86</v>
       </c>
@@ -7664,14 +8402,17 @@
         <v>Dl 26504</v>
       </c>
       <c r="E36" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
         <v>r_dl_26504</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>90</v>
       </c>
@@ -7683,14 +8424,17 @@
         <v>Dl 31394</v>
       </c>
       <c r="E37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
         <v>r_dl_31394</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>8</v>
       </c>
@@ -7702,14 +8446,17 @@
         <v>Dl 21899 Y 21394</v>
       </c>
       <c r="E38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="1"/>
         <v>r_dl_21899_21394</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
         <v>117</v>
       </c>
@@ -7721,14 +8468,17 @@
         <v>Ds 257-59</v>
       </c>
       <c r="E39" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_25759</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
         <v>248</v>
       </c>
@@ -7740,14 +8490,17 @@
         <v>Ds 38-87</v>
       </c>
       <c r="E40" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_3887</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
         <v>7</v>
       </c>
@@ -7759,14 +8512,17 @@
         <v>Ds 031-88</v>
       </c>
       <c r="E41" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_03188</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>79</v>
       </c>
@@ -7778,14 +8534,17 @@
         <v>Ds 155-88</v>
       </c>
       <c r="E42" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_15588</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>5</v>
       </c>
@@ -7797,14 +8556,17 @@
         <v>Ds 132-89</v>
       </c>
       <c r="E43" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_13289</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
         <v>214</v>
       </c>
@@ -7816,14 +8578,17 @@
         <v>Ds 285-89</v>
       </c>
       <c r="E44" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_28589</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
         <v>55</v>
       </c>
@@ -7835,14 +8600,17 @@
         <v>Ds 051-91</v>
       </c>
       <c r="E45" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_05191</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>74</v>
       </c>
@@ -7854,14 +8622,17 @@
         <v>Ds 276-91</v>
       </c>
       <c r="E46" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_27691</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
         <v>222</v>
       </c>
@@ -7873,14 +8644,17 @@
         <v>Du 37-94</v>
       </c>
       <c r="E47" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="1"/>
         <v>r_du_3794</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
         <v>196</v>
       </c>
@@ -7892,14 +8666,17 @@
         <v>Du 90-96</v>
       </c>
       <c r="E48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="1"/>
         <v>r_du_9096</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
         <v>83</v>
       </c>
@@ -7911,14 +8688,17 @@
         <v>Ds 256-97</v>
       </c>
       <c r="E49" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_25697</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
         <v>183</v>
       </c>
@@ -7930,14 +8710,17 @@
         <v>Du 73-97</v>
       </c>
       <c r="E50" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="1"/>
         <v>r_du_7397</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
         <v>252</v>
       </c>
@@ -7949,14 +8732,17 @@
         <v>Du 011-99</v>
       </c>
       <c r="E51" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="1"/>
         <v>r_du_01199</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
         <v>4</v>
       </c>
@@ -7968,14 +8754,17 @@
         <v>Ds 16-05</v>
       </c>
       <c r="E52" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_1605</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
         <v>162</v>
       </c>
@@ -7987,14 +8776,17 @@
         <v>Ds 17-05</v>
       </c>
       <c r="E53" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_1705</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
         <v>119</v>
       </c>
@@ -8006,14 +8798,17 @@
         <v>Ds 110-06</v>
       </c>
       <c r="E54" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_11006</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>88</v>
       </c>
@@ -8025,14 +8820,17 @@
         <v>Ds 39-07</v>
       </c>
       <c r="E55" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_3907</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
         <v>92</v>
       </c>
@@ -8044,14 +8842,17 @@
         <v>Ds 120-08</v>
       </c>
       <c r="E56" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_12008</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
         <v>163</v>
       </c>
@@ -8063,24 +8864,27 @@
         <v>Ds 14-09</v>
       </c>
       <c r="E57" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="1"/>
         <v>r_ds_1409</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="29" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
     </row>
   </sheetData>
@@ -8094,14 +8898,14 @@
       <formula>"CONTAR.SI($C:$C, A2) &gt; 0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:D2 C33:C39 C58:D1048576 C41:C57 D3:D57">
-    <cfRule type="expression" dxfId="3" priority="20">
-      <formula>"CONTAR.SI($A:$A, C1) &gt; 0"</formula>
+  <conditionalFormatting sqref="C3:C57">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>"CONTAR.SI($C:$C, A2) &gt; 0"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C57">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>"CONTAR.SI($C:$C, A2) &gt; 0"</formula>
+  <conditionalFormatting sqref="C1:D2 D3:D57 C33:C39 C41:C57 C58:D1048576">
+    <cfRule type="expression" dxfId="2" priority="20">
+      <formula>"CONTAR.SI($A:$A, C1) &gt; 0"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8110,20 +8914,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2FD9B8-B3D0-4C0E-9CB6-FE83D514A81F}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>289</v>
       </c>
@@ -8131,7 +8937,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>21</v>
       </c>
@@ -8141,8 +8947,22 @@
       <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>PROPER(C2)</f>
+        <v>Adelanto Sueldo</v>
+      </c>
+      <c r="E2" t="s">
+        <v>484</v>
+      </c>
+      <c r="F2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT("dh_",F2)</f>
+        <v>dh_adelanto_sueldo</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>283</v>
       </c>
@@ -8152,8 +8972,22 @@
       <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:E58" si="0">PROPER(C3)</f>
+        <v>Buena Cuenta</v>
+      </c>
+      <c r="E3" t="s">
+        <v>485</v>
+      </c>
+      <c r="F3" t="s">
+        <v>428</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G58" si="1">_xlfn.CONCAT("dh_",F3)</f>
+        <v>dh_buena_cuenta</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -8163,8 +8997,22 @@
       <c r="C4" s="5" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Caja Pensiones</v>
+      </c>
+      <c r="E4" t="s">
+        <v>533</v>
+      </c>
+      <c r="F4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_caja_pen</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>313</v>
       </c>
@@ -8174,8 +9022,22 @@
       <c r="C5" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Caja Pensiones 1%</v>
+      </c>
+      <c r="E5" t="s">
+        <v>532</v>
+      </c>
+      <c r="F5" t="s">
+        <v>465</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_caja_pen_1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
@@ -8185,8 +9047,22 @@
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Caja Pensiones 3%</v>
+      </c>
+      <c r="E6" t="s">
+        <v>534</v>
+      </c>
+      <c r="F6" t="s">
+        <v>466</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_caja_pen_3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -8196,8 +9072,22 @@
       <c r="C7" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Cuarta Cat</v>
+      </c>
+      <c r="E7" t="s">
+        <v>486</v>
+      </c>
+      <c r="F7" t="s">
+        <v>429</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_cuarta_cat</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>287</v>
       </c>
@@ -8207,8 +9097,22 @@
       <c r="C8" s="35" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Quinta Cat</v>
+      </c>
+      <c r="E8" t="s">
+        <v>487</v>
+      </c>
+      <c r="F8" t="s">
+        <v>433</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_quinta_cat</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>98</v>
       </c>
@@ -8218,8 +9122,22 @@
       <c r="C9" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Derrama Adm</v>
+      </c>
+      <c r="E9" t="s">
+        <v>488</v>
+      </c>
+      <c r="F9" t="s">
+        <v>430</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_derrama_adm</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>154</v>
       </c>
@@ -8229,8 +9147,22 @@
       <c r="C10" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Desc Vol</v>
+      </c>
+      <c r="E10" t="s">
+        <v>489</v>
+      </c>
+      <c r="F10" t="s">
+        <v>440</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_voluntario</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>66</v>
       </c>
@@ -8240,8 +9172,22 @@
       <c r="C11" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Descuento Judicial</v>
+      </c>
+      <c r="E11" t="s">
+        <v>535</v>
+      </c>
+      <c r="F11" t="s">
+        <v>439</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_judicial</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>216</v>
       </c>
@@ -8251,8 +9197,22 @@
       <c r="C12" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Falta Y Tardanza</v>
+      </c>
+      <c r="E12" t="s">
+        <v>536</v>
+      </c>
+      <c r="F12" t="s">
+        <v>467</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_falta_tard</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>146</v>
       </c>
@@ -8262,8 +9222,22 @@
       <c r="C13" s="34" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Fon 1%</v>
+      </c>
+      <c r="E13" t="s">
+        <v>490</v>
+      </c>
+      <c r="F13" t="s">
+        <v>441</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fonavi_1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>110</v>
       </c>
@@ -8273,8 +9247,22 @@
       <c r="C14" s="34" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Fonavi</v>
+      </c>
+      <c r="E14" t="s">
+        <v>491</v>
+      </c>
+      <c r="F14" t="s">
+        <v>333</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fonavi</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>130</v>
       </c>
@@ -8284,8 +9272,22 @@
       <c r="C15" s="34" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Fonavi 0.5%</v>
+      </c>
+      <c r="E15" t="s">
+        <v>492</v>
+      </c>
+      <c r="F15" t="s">
+        <v>443</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fonavi_05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
@@ -8295,8 +9297,22 @@
       <c r="C16" s="29" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Fondo</v>
+      </c>
+      <c r="E16" t="s">
+        <v>493</v>
+      </c>
+      <c r="F16" t="s">
+        <v>442</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fondo</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>190</v>
       </c>
@@ -8306,8 +9322,22 @@
       <c r="C17" s="29" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Fondo 10%</v>
+      </c>
+      <c r="E17" t="s">
+        <v>494</v>
+      </c>
+      <c r="F17" t="s">
+        <v>444</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fondo_10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>117</v>
       </c>
@@ -8317,8 +9347,22 @@
       <c r="C18" s="29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Fondo Pensiones 6%</v>
+      </c>
+      <c r="E18" t="s">
+        <v>495</v>
+      </c>
+      <c r="F18" t="s">
+        <v>468</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fondo_pen_6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>147</v>
       </c>
@@ -8328,8 +9372,22 @@
       <c r="C19" s="29" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Fondo Pensiones 8-4-7%</v>
+      </c>
+      <c r="E19" t="s">
+        <v>496</v>
+      </c>
+      <c r="F19" t="s">
+        <v>469</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fondo_pen_847</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
         <v>220</v>
       </c>
@@ -8339,8 +9397,22 @@
       <c r="C20" s="29" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Fondo Spp 8%</v>
+      </c>
+      <c r="E20" t="s">
+        <v>497</v>
+      </c>
+      <c r="F20" t="s">
+        <v>445</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fondo_spp_8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>258</v>
       </c>
@@ -8350,8 +9422,22 @@
       <c r="C21" s="29" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Fondo-Spp</v>
+      </c>
+      <c r="E21" t="s">
+        <v>498</v>
+      </c>
+      <c r="F21" t="s">
+        <v>432</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_fondo_spp</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>14</v>
       </c>
@@ -8361,8 +9447,22 @@
       <c r="C22" s="29" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Aporte Afp</v>
+      </c>
+      <c r="E22" t="s">
+        <v>499</v>
+      </c>
+      <c r="F22" t="s">
+        <v>427</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_aporte_afp</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>94</v>
       </c>
@@ -8372,8 +9472,22 @@
       <c r="C23" s="29" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Dev Afp</v>
+      </c>
+      <c r="E23" t="s">
+        <v>500</v>
+      </c>
+      <c r="F23" t="s">
+        <v>431</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_dev_afp</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
         <v>250</v>
       </c>
@@ -8383,8 +9497,22 @@
       <c r="C24" s="29" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Pll Afp</v>
+      </c>
+      <c r="E24" t="s">
+        <v>501</v>
+      </c>
+      <c r="F24" t="s">
+        <v>434</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_pll_afp</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
         <v>242</v>
       </c>
@@ -8394,8 +9522,22 @@
       <c r="C25" s="29" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>R Afp</v>
+      </c>
+      <c r="E25" t="s">
+        <v>502</v>
+      </c>
+      <c r="F25" t="s">
+        <v>435</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_r_afp</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
@@ -8405,8 +9547,22 @@
       <c r="C26" s="29" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Retencion</v>
+      </c>
+      <c r="E26" t="s">
+        <v>503</v>
+      </c>
+      <c r="F26" t="s">
+        <v>470</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ret</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>60</v>
       </c>
@@ -8416,8 +9572,22 @@
       <c r="C27" s="29" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>Retencion Afp</v>
+      </c>
+      <c r="E27" t="s">
+        <v>504</v>
+      </c>
+      <c r="F27" t="s">
+        <v>471</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ret_afp</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>79</v>
       </c>
@@ -8427,8 +9597,22 @@
       <c r="C28" s="36" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp</v>
+      </c>
+      <c r="E28" t="s">
+        <v>505</v>
+      </c>
+      <c r="F28" t="s">
+        <v>446</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_snp</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>20</v>
       </c>
@@ -8438,8 +9622,22 @@
       <c r="C29" s="36" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 2%</v>
+      </c>
+      <c r="E29" t="s">
+        <v>506</v>
+      </c>
+      <c r="F29" t="s">
+        <v>473</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_snp_2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>132</v>
       </c>
@@ -8449,8 +9647,22 @@
       <c r="C30" s="36" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 2.5%</v>
+      </c>
+      <c r="E30" t="s">
+        <v>507</v>
+      </c>
+      <c r="F30" t="s">
+        <v>447</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_snp_25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>19</v>
       </c>
@@ -8460,8 +9672,22 @@
       <c r="C31" s="36" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 3%</v>
+      </c>
+      <c r="E31" t="s">
+        <v>508</v>
+      </c>
+      <c r="F31" t="s">
+        <v>448</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_snp_3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>205</v>
       </c>
@@ -8471,8 +9697,22 @@
       <c r="C32" s="36" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 11%</v>
+      </c>
+      <c r="E32" t="s">
+        <v>509</v>
+      </c>
+      <c r="F32" t="s">
+        <v>449</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_snp_11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>310</v>
       </c>
@@ -8482,8 +9722,22 @@
       <c r="C33" s="36" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 13%</v>
+      </c>
+      <c r="E33" t="s">
+        <v>510</v>
+      </c>
+      <c r="F33" t="s">
+        <v>450</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_snp_13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>311</v>
       </c>
@@ -8493,8 +9747,22 @@
       <c r="C34" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Goce 6%</v>
+      </c>
+      <c r="E34" t="s">
+        <v>511</v>
+      </c>
+      <c r="F34" t="s">
+        <v>451</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_goce_6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>312</v>
       </c>
@@ -8504,8 +9772,22 @@
       <c r="C35" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>Goce 8%</v>
+      </c>
+      <c r="E35" t="s">
+        <v>512</v>
+      </c>
+      <c r="F35" t="s">
+        <v>452</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_goce_8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>309</v>
       </c>
@@ -8515,8 +9797,22 @@
       <c r="C36" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>Gratificacion</v>
+      </c>
+      <c r="E36" t="s">
+        <v>513</v>
+      </c>
+      <c r="F36" t="s">
+        <v>472</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_grati</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>126</v>
       </c>
@@ -8526,8 +9822,22 @@
       <c r="C37" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>Grav Nombram</v>
+      </c>
+      <c r="E37" t="s">
+        <v>514</v>
+      </c>
+      <c r="F37" t="s">
+        <v>474</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_grav_nomb</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
         <v>260</v>
       </c>
@@ -8537,8 +9847,22 @@
       <c r="C38" s="5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>Imp Rent</v>
+      </c>
+      <c r="E38" t="s">
+        <v>515</v>
+      </c>
+      <c r="F38" t="s">
+        <v>436</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_imp_rent</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>96</v>
       </c>
@@ -8548,8 +9872,22 @@
       <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Impuesto Sueldo</v>
+      </c>
+      <c r="E39" t="s">
+        <v>516</v>
+      </c>
+      <c r="F39" t="s">
+        <v>475</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_imp_sueldo</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>25</v>
       </c>
@@ -8559,8 +9897,22 @@
       <c r="C40" s="5" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>Ips</v>
+      </c>
+      <c r="E40" t="s">
+        <v>517</v>
+      </c>
+      <c r="F40" t="s">
+        <v>453</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ips</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>100</v>
       </c>
@@ -8570,8 +9922,22 @@
       <c r="C41" s="5" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Ips 2.5%</v>
+      </c>
+      <c r="E41" t="s">
+        <v>518</v>
+      </c>
+      <c r="F41" t="s">
+        <v>454</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ips_25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>218</v>
       </c>
@@ -8581,8 +9947,22 @@
       <c r="C42" s="5" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>Ips 3%</v>
+      </c>
+      <c r="E42" t="s">
+        <v>519</v>
+      </c>
+      <c r="F42" t="s">
+        <v>455</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ips_3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
         <v>261</v>
       </c>
@@ -8592,8 +9972,22 @@
       <c r="C43" s="5" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>Ips 4%</v>
+      </c>
+      <c r="E43" t="s">
+        <v>520</v>
+      </c>
+      <c r="F43" t="s">
+        <v>456</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ips_4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
         <v>284</v>
       </c>
@@ -8603,8 +9997,22 @@
       <c r="C44" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>Montepio</v>
+      </c>
+      <c r="E44" t="s">
+        <v>521</v>
+      </c>
+      <c r="F44" t="s">
+        <v>457</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_montepio</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>15</v>
       </c>
@@ -8614,8 +10022,22 @@
       <c r="C45" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>Prestamo Adm</v>
+      </c>
+      <c r="E45" t="s">
+        <v>522</v>
+      </c>
+      <c r="F45" t="s">
+        <v>437</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_prestamo_adm</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>16</v>
       </c>
@@ -8625,8 +10047,22 @@
       <c r="C46" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>Quincena</v>
+      </c>
+      <c r="E46" t="s">
+        <v>523</v>
+      </c>
+      <c r="F46" t="s">
+        <v>458</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_quincena</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>63</v>
       </c>
@@ -8636,8 +10072,22 @@
       <c r="C47" s="33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Seguro Social</v>
+      </c>
+      <c r="E47" t="s">
+        <v>537</v>
+      </c>
+      <c r="F47" t="s">
+        <v>476</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_seg_soc</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="33" t="s">
         <v>24</v>
       </c>
@@ -8647,8 +10097,22 @@
       <c r="C48" s="33" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>Seguro Social 1.5%</v>
+      </c>
+      <c r="E48" t="s">
+        <v>538</v>
+      </c>
+      <c r="F48" t="s">
+        <v>477</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_seg_soc_15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
         <v>230</v>
       </c>
@@ -8658,8 +10122,22 @@
       <c r="C49" s="33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>Seguro Social 2.1%</v>
+      </c>
+      <c r="E49" t="s">
+        <v>539</v>
+      </c>
+      <c r="F49" t="s">
+        <v>478</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_seg_soc_21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="29" t="s">
         <v>150</v>
       </c>
@@ -8669,8 +10147,22 @@
       <c r="C50" s="33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>Seguro Social 2.5%</v>
+      </c>
+      <c r="E50" t="s">
+        <v>540</v>
+      </c>
+      <c r="F50" t="s">
+        <v>479</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_seg_soc_25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
         <v>228</v>
       </c>
@@ -8680,8 +10172,22 @@
       <c r="C51" s="33" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>Seguro Vida</v>
+      </c>
+      <c r="E51" t="s">
+        <v>524</v>
+      </c>
+      <c r="F51" t="s">
+        <v>480</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_seg_vida</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="29" t="s">
         <v>235</v>
       </c>
@@ -8691,8 +10197,22 @@
       <c r="C52" s="5" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>Tesoreria</v>
+      </c>
+      <c r="E52" t="s">
+        <v>525</v>
+      </c>
+      <c r="F52" t="s">
+        <v>459</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_tesoreria</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="29" t="s">
         <v>102</v>
       </c>
@@ -8702,8 +10222,22 @@
       <c r="C53" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>Vacaciones</v>
+      </c>
+      <c r="E53" t="s">
+        <v>526</v>
+      </c>
+      <c r="F53" t="s">
+        <v>481</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_vacac</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="29" t="s">
         <v>135</v>
       </c>
@@ -8713,8 +10247,22 @@
       <c r="C54" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>Viaticos</v>
+      </c>
+      <c r="E54" t="s">
+        <v>527</v>
+      </c>
+      <c r="F54" t="s">
+        <v>342</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_viaticos</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="29" t="s">
         <v>192</v>
       </c>
@@ -8724,8 +10272,22 @@
       <c r="C55" s="5" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>Ley 7904</v>
+      </c>
+      <c r="E55" t="s">
+        <v>528</v>
+      </c>
+      <c r="F55" t="s">
+        <v>460</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ley_7904</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>137</v>
       </c>
@@ -8735,8 +10297,22 @@
       <c r="C56" s="5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>Dl 20530</v>
+      </c>
+      <c r="E56" t="s">
+        <v>529</v>
+      </c>
+      <c r="F56" t="s">
+        <v>461</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_dl_20530</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>26</v>
       </c>
@@ -8746,8 +10322,22 @@
       <c r="C57" s="5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>Dl 22161</v>
+      </c>
+      <c r="E57" t="s">
+        <v>530</v>
+      </c>
+      <c r="F57" t="s">
+        <v>462</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_dl_22161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>58</v>
       </c>
@@ -8756,6 +10346,20 @@
       </c>
       <c r="C58" s="5" t="s">
         <v>130</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>Ds 043</v>
+      </c>
+      <c r="E58" t="s">
+        <v>531</v>
+      </c>
+      <c r="F58" t="s">
+        <v>463</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v>dh_ds_043</v>
       </c>
     </row>
   </sheetData>
@@ -8775,27 +10379,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1569F0-E1B8-4AFD-A657-CFE06B4DD5BE}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E2" sqref="E2:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>583</v>
+      </c>
+      <c r="G1" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -8805,8 +10416,22 @@
       <c r="C2" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f>PROPER(C2)</f>
+        <v>Ss Cuota Patronal</v>
+      </c>
+      <c r="E2" t="s">
+        <v>561</v>
+      </c>
+      <c r="F2" t="s">
+        <v>563</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT("ah_",F2)</f>
+        <v>ah_ss_cuota_pat</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>202</v>
       </c>
@@ -8816,8 +10441,22 @@
       <c r="C3" s="5" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:E26" si="0">PROPER(C3)</f>
+        <v>Cp Cuota Patronal</v>
+      </c>
+      <c r="E3" t="s">
+        <v>562</v>
+      </c>
+      <c r="F3" t="s">
+        <v>564</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G26" si="1">_xlfn.CONCAT("ah_",F3)</f>
+        <v>ah_cp_cuota_pat</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
@@ -8827,8 +10466,22 @@
       <c r="C4" s="19" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Caja Pens</v>
+      </c>
+      <c r="E4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F4" t="s">
+        <v>565</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_caja_pens</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>121</v>
       </c>
@@ -8838,8 +10491,22 @@
       <c r="C5" s="20" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Cem 3%</v>
+      </c>
+      <c r="E5" t="s">
+        <v>542</v>
+      </c>
+      <c r="F5" t="s">
+        <v>566</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_cem_3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>123</v>
       </c>
@@ -8849,8 +10516,22 @@
       <c r="C6" s="20" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Cem 5%</v>
+      </c>
+      <c r="E6" t="s">
+        <v>543</v>
+      </c>
+      <c r="F6" t="s">
+        <v>567</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_cem_5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>140</v>
       </c>
@@ -8860,8 +10541,22 @@
       <c r="C7" s="20" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Cen</v>
+      </c>
+      <c r="E7" t="s">
+        <v>544</v>
+      </c>
+      <c r="F7" t="s">
+        <v>581</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_cen</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>143</v>
       </c>
@@ -8871,8 +10566,22 @@
       <c r="C8" s="20" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Cen 5%</v>
+      </c>
+      <c r="E8" t="s">
+        <v>545</v>
+      </c>
+      <c r="F8" t="s">
+        <v>568</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_cen_5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>141</v>
       </c>
@@ -8882,8 +10591,22 @@
       <c r="C9" s="20" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Cen 6%</v>
+      </c>
+      <c r="E9" t="s">
+        <v>546</v>
+      </c>
+      <c r="F9" t="s">
+        <v>569</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_cen_6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>146</v>
       </c>
@@ -8893,8 +10616,22 @@
       <c r="C10" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Seg Soc</v>
+      </c>
+      <c r="E10" t="s">
+        <v>547</v>
+      </c>
+      <c r="F10" t="s">
+        <v>476</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_seg_soc</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>203</v>
       </c>
@@ -8904,8 +10641,22 @@
       <c r="C11" s="20" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Essalud 9%</v>
+      </c>
+      <c r="E11" t="s">
+        <v>548</v>
+      </c>
+      <c r="F11" t="s">
+        <v>570</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_essalud_9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>156</v>
       </c>
@@ -8915,8 +10666,22 @@
       <c r="C12" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Fonavi</v>
+      </c>
+      <c r="E12" t="s">
+        <v>491</v>
+      </c>
+      <c r="F12" t="s">
+        <v>333</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_fonavi</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>158</v>
       </c>
@@ -8926,8 +10691,22 @@
       <c r="C13" s="20" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Fon 4%</v>
+      </c>
+      <c r="E13" t="s">
+        <v>549</v>
+      </c>
+      <c r="F13" t="s">
+        <v>571</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_fon_4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>159</v>
       </c>
@@ -8937,8 +10716,22 @@
       <c r="C14" s="20" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Fon 5%</v>
+      </c>
+      <c r="E14" t="s">
+        <v>550</v>
+      </c>
+      <c r="F14" t="s">
+        <v>572</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_fon_5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>168</v>
       </c>
@@ -8948,8 +10741,22 @@
       <c r="C15" s="20" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Fon 8%</v>
+      </c>
+      <c r="E15" t="s">
+        <v>551</v>
+      </c>
+      <c r="F15" t="s">
+        <v>573</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_fon_8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>150</v>
       </c>
@@ -8959,8 +10766,22 @@
       <c r="C16" s="20" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Fon 9%</v>
+      </c>
+      <c r="E16" t="s">
+        <v>552</v>
+      </c>
+      <c r="F16" t="s">
+        <v>574</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_fon_9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>166</v>
       </c>
@@ -8970,8 +10791,22 @@
       <c r="C17" s="20" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Fon 7%</v>
+      </c>
+      <c r="E17" t="s">
+        <v>553</v>
+      </c>
+      <c r="F17" t="s">
+        <v>575</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_fon_7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>186</v>
       </c>
@@ -8981,8 +10816,22 @@
       <c r="C18" s="20" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Ipss</v>
+      </c>
+      <c r="E18" t="s">
+        <v>554</v>
+      </c>
+      <c r="F18" t="s">
+        <v>582</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_ipss</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>188</v>
       </c>
@@ -8992,8 +10841,22 @@
       <c r="C19" s="20" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ies 1.7%</v>
+      </c>
+      <c r="E19" t="s">
+        <v>555</v>
+      </c>
+      <c r="F19" t="s">
+        <v>576</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_ies_7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>204</v>
       </c>
@@ -9003,8 +10866,22 @@
       <c r="C20" s="20" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Ies 2%</v>
+      </c>
+      <c r="E20" t="s">
+        <v>556</v>
+      </c>
+      <c r="F20" t="s">
+        <v>577</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_ies_2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>226</v>
       </c>
@@ -9014,8 +10891,22 @@
       <c r="C21" s="20" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Ipss 6%</v>
+      </c>
+      <c r="E21" t="s">
+        <v>557</v>
+      </c>
+      <c r="F21" t="s">
+        <v>578</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_ipss_6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>224</v>
       </c>
@@ -9025,8 +10916,22 @@
       <c r="C22" s="20" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Ipss 9%</v>
+      </c>
+      <c r="E22" t="s">
+        <v>558</v>
+      </c>
+      <c r="F22" t="s">
+        <v>579</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_ipss_9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>232</v>
       </c>
@@ -9036,8 +10941,22 @@
       <c r="C23" s="20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp</v>
+      </c>
+      <c r="E23" t="s">
+        <v>505</v>
+      </c>
+      <c r="F23" t="s">
+        <v>446</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_snp</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>240</v>
       </c>
@@ -9047,8 +10966,22 @@
       <c r="C24" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 5%</v>
+      </c>
+      <c r="E24" t="s">
+        <v>559</v>
+      </c>
+      <c r="F24" t="s">
+        <v>438</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_snp_5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>246</v>
       </c>
@@ -9058,8 +10991,22 @@
       <c r="C25" s="20" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Snp 6%</v>
+      </c>
+      <c r="E25" t="s">
+        <v>560</v>
+      </c>
+      <c r="F25" t="s">
+        <v>580</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_snp_6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>244</v>
       </c>
@@ -9068,6 +11015,20 @@
       </c>
       <c r="C26" s="20" t="s">
         <v>146</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Dl 20530</v>
+      </c>
+      <c r="E26" t="s">
+        <v>529</v>
+      </c>
+      <c r="F26" t="s">
+        <v>461</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>ah_dl_20530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>